<commit_message>
Corrected calculation of thrust constant for all rotors.
</commit_message>
<xml_diff>
--- a/tests/rotor3/Rotor3_Thrust_Constant_Calculation.xlsx
+++ b/tests/rotor3/Rotor3_Thrust_Constant_Calculation.xlsx
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fer\repos\rx-2\tests\rotor3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE4B699-866A-448D-BB1E-E4BE3D23D7A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA63C240-E4ED-4C8B-9AE0-1C5DE88CB810}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10770" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rotor2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Force {N} (mean)</t>
   </si>
@@ -44,6 +52,9 @@
   </si>
   <si>
     <t>Rotor 3 Thrust Test 5</t>
+  </si>
+  <si>
+    <t>offset</t>
   </si>
 </sst>
 </file>
@@ -746,8 +757,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -764,16 +775,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -969,121 +990,121 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$C$3:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$A$3:$A$37</c:f>
               <c:numCache>
@@ -1196,7 +1217,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1219,132 +1240,142 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$C$3:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$B$3:$B$37</c:f>
               <c:numCache>
@@ -1457,7 +1488,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1473,11 +1504,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="134086735"/>
         <c:axId val="71346895"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="134086735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1523,11 +1553,8 @@
         </c:txPr>
         <c:crossAx val="71346895"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="71346895"/>
         <c:scaling>
@@ -1582,7 +1609,7 @@
         </c:txPr>
         <c:crossAx val="134086735"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1746,8 +1773,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1764,16 +1791,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -1827,121 +1864,121 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$I$3:$I$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$G$3:$G$37</c:f>
               <c:numCache>
@@ -2054,7 +2091,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2077,132 +2114,142 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$I$3:$I$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$H$3:$H$37</c:f>
               <c:numCache>
@@ -2315,7 +2362,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2331,11 +2378,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="243341903"/>
         <c:axId val="149250335"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="243341903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -2381,11 +2427,8 @@
         </c:txPr>
         <c:crossAx val="149250335"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="149250335"/>
         <c:scaling>
@@ -2440,7 +2483,7 @@
         </c:txPr>
         <c:crossAx val="243341903"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2597,8 +2640,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2615,16 +2658,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -2644,8 +2697,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43400459317585299"/>
-                  <c:y val="4.9586249635462237E-2"/>
+                  <c:x val="-0.25664527013467175"/>
+                  <c:y val="4.6398952299853578E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2678,121 +2731,121 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$F$3:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$D$3:$D$37</c:f>
               <c:numCache>
@@ -2905,7 +2958,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2928,132 +2981,142 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$F$3:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$E$3:$E$37</c:f>
               <c:numCache>
@@ -3166,7 +3229,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3182,11 +3245,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="134076335"/>
         <c:axId val="149268639"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="134076335"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -3232,11 +3294,8 @@
         </c:txPr>
         <c:crossAx val="149268639"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="149268639"/>
         <c:scaling>
@@ -3291,7 +3350,7 @@
         </c:txPr>
         <c:crossAx val="134076335"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3455,8 +3514,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -3473,16 +3532,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -3536,121 +3605,121 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$L$3:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$J$3:$J$37</c:f>
               <c:numCache>
@@ -3763,7 +3832,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3786,132 +3855,142 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$L$3:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$K$3:$K$37</c:f>
               <c:numCache>
@@ -4024,7 +4103,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4040,11 +4119,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="243389103"/>
         <c:axId val="62806815"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="243389103"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -4090,11 +4168,8 @@
         </c:txPr>
         <c:crossAx val="62806815"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="62806815"/>
         <c:scaling>
@@ -4149,7 +4224,7 @@
         </c:txPr>
         <c:crossAx val="243389103"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4321,8 +4396,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -4339,16 +4414,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -4402,121 +4487,121 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$O$3:$O$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$M$3:$M$37</c:f>
               <c:numCache>
@@ -4629,7 +4714,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4652,132 +4737,142 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Rotor2!$O$3:$O$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999899</c:v>
+                  <c:v>9.9999999999989875E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999904</c:v>
+                  <c:v>0.19999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2999999999999901</c:v>
+                  <c:v>0.29999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3999999999999897</c:v>
+                  <c:v>0.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4999999999999902</c:v>
+                  <c:v>0.49999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5999999999999899</c:v>
+                  <c:v>0.59999999999998987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6999999999999904</c:v>
+                  <c:v>0.69999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7999999999999901</c:v>
+                  <c:v>0.79999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8999999999999897</c:v>
+                  <c:v>0.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9999999999999902</c:v>
+                  <c:v>0.99999999999999023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0999999999999899</c:v>
+                  <c:v>1.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.1999999999999904</c:v>
+                  <c:v>1.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2999999999999901</c:v>
+                  <c:v>1.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3999999999999897</c:v>
+                  <c:v>1.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4999999999999902</c:v>
+                  <c:v>1.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5999999999999899</c:v>
+                  <c:v>1.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6999999999999904</c:v>
+                  <c:v>1.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7999999999999901</c:v>
+                  <c:v>1.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8999999999999897</c:v>
+                  <c:v>1.8999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9999999999999902</c:v>
+                  <c:v>1.9999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0999999999999899</c:v>
+                  <c:v>2.0999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1999999999999904</c:v>
+                  <c:v>2.1999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2999999999999901</c:v>
+                  <c:v>2.2999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3999999999999897</c:v>
+                  <c:v>2.3999999999999897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4999999999999902</c:v>
+                  <c:v>2.4999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.5999999999999899</c:v>
+                  <c:v>2.5999999999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.6999999999999904</c:v>
+                  <c:v>2.6999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7999999999999901</c:v>
+                  <c:v>2.7999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8999999999999799</c:v>
+                  <c:v>2.8999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.9999999999999796</c:v>
+                  <c:v>2.9999999999999796</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.0999999999999801</c:v>
+                  <c:v>3.0999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.1999999999999797</c:v>
+                  <c:v>3.1999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.2999999999999794</c:v>
+                  <c:v>3.2999999999999794</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3999999999999808</c:v>
+                  <c:v>3.3999999999999808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Rotor2!$N$3:$N$37</c:f>
               <c:numCache>
@@ -4890,7 +4985,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4906,11 +5001,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="247911263"/>
         <c:axId val="251369759"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="247911263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -4956,11 +5050,8 @@
         </c:txPr>
         <c:crossAx val="251369759"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="251369759"/>
         <c:scaling>
@@ -5015,7 +5106,7 @@
         </c:txPr>
         <c:crossAx val="247911263"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -8362,15 +8453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -8397,7 +8488,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8444,7 +8535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -8452,7 +8543,8 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <f>P3-$B$38</f>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -8461,7 +8553,8 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <f>P3-$B$38</f>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -8470,7 +8563,8 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <f>P3-$B$38</f>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -8479,7 +8573,8 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <f>P3-$B$38</f>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -8488,10 +8583,14 @@
         <v>0</v>
       </c>
       <c r="O3">
+        <f>P3-$B$38</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -8499,7 +8598,8 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5.0999999999999899</v>
+        <f t="shared" ref="C4:C37" si="0">P4-$B$38</f>
+        <v>9.9999999999989875E-2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -8508,7 +8608,8 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>5.0999999999999899</v>
+        <f t="shared" ref="F4:F37" si="1">P4-$B$38</f>
+        <v>9.9999999999989875E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -8517,7 +8618,8 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>5.0999999999999899</v>
+        <f t="shared" ref="I4:I37" si="2">P4-$B$38</f>
+        <v>9.9999999999989875E-2</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -8526,7 +8628,8 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>5.0999999999999899</v>
+        <f t="shared" ref="L4:L37" si="3">P4-$B$38</f>
+        <v>9.9999999999989875E-2</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -8535,10 +8638,14 @@
         <v>0</v>
       </c>
       <c r="O4">
+        <f t="shared" ref="O4:O37" si="4">P4-$B$38</f>
+        <v>9.9999999999989875E-2</v>
+      </c>
+      <c r="P4">
         <v>5.0999999999999899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -8546,7 +8653,8 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5.1999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>0.19999999999999041</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -8555,7 +8663,8 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>5.1999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>0.19999999999999041</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -8564,7 +8673,8 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>5.1999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>0.19999999999999041</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -8573,7 +8683,8 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>5.1999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>0.19999999999999041</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -8582,10 +8693,14 @@
         <v>0</v>
       </c>
       <c r="O5">
+        <f t="shared" si="4"/>
+        <v>0.19999999999999041</v>
+      </c>
+      <c r="P5">
         <v>5.1999999999999904</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -8593,7 +8708,8 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>5.2999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>0.29999999999999005</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -8602,7 +8718,8 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>5.2999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>0.29999999999999005</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -8611,7 +8728,8 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>5.2999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>0.29999999999999005</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -8620,7 +8738,8 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>5.2999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>0.29999999999999005</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -8629,10 +8748,14 @@
         <v>0</v>
       </c>
       <c r="O6">
+        <f t="shared" si="4"/>
+        <v>0.29999999999999005</v>
+      </c>
+      <c r="P6">
         <v>5.2999999999999901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.127999999999999</v>
       </c>
@@ -8640,7 +8763,8 @@
         <v>4.1039134083406103E-3</v>
       </c>
       <c r="C7">
-        <v>5.3999999999999897</v>
+        <f t="shared" si="0"/>
+        <v>0.3999999999999897</v>
       </c>
       <c r="D7">
         <v>0.13250000000000001</v>
@@ -8649,7 +8773,8 @@
         <v>7.1635039941137903E-3</v>
       </c>
       <c r="F7">
-        <v>5.3999999999999897</v>
+        <f t="shared" si="1"/>
+        <v>0.3999999999999897</v>
       </c>
       <c r="G7">
         <v>0.14599999999999999</v>
@@ -8658,7 +8783,8 @@
         <v>6.8055704737871904E-3</v>
       </c>
       <c r="I7">
-        <v>5.3999999999999897</v>
+        <f t="shared" si="2"/>
+        <v>0.3999999999999897</v>
       </c>
       <c r="J7">
         <v>0.14699999999999899</v>
@@ -8667,7 +8793,8 @@
         <v>2.3418391333129101E-2</v>
       </c>
       <c r="L7">
-        <v>5.3999999999999897</v>
+        <f t="shared" si="3"/>
+        <v>0.3999999999999897</v>
       </c>
       <c r="M7">
         <v>0.155</v>
@@ -8676,10 +8803,14 @@
         <v>1.10023920844036E-2</v>
       </c>
       <c r="O7">
+        <f t="shared" si="4"/>
+        <v>0.3999999999999897</v>
+      </c>
+      <c r="P7">
         <v>5.3999999999999897</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.28399999999999997</v>
       </c>
@@ -8687,7 +8818,8 @@
         <v>8.2078268166812102E-3</v>
       </c>
       <c r="C8">
-        <v>5.4999999999999902</v>
+        <f t="shared" si="0"/>
+        <v>0.49999999999999023</v>
       </c>
       <c r="D8">
         <v>0.26199999999999901</v>
@@ -8696,7 +8828,8 @@
         <v>8.9442719099991595E-3</v>
       </c>
       <c r="F8">
-        <v>5.4999999999999902</v>
+        <f t="shared" si="1"/>
+        <v>0.49999999999999023</v>
       </c>
       <c r="G8">
         <v>0.246</v>
@@ -8705,7 +8838,8 @@
         <v>8.8257995015808798E-3</v>
       </c>
       <c r="I8">
-        <v>5.4999999999999902</v>
+        <f t="shared" si="2"/>
+        <v>0.49999999999999023</v>
       </c>
       <c r="J8">
         <v>0.310499999999999</v>
@@ -8714,7 +8848,8 @@
         <v>4.3706557378667202E-2</v>
       </c>
       <c r="L8">
-        <v>5.4999999999999902</v>
+        <f t="shared" si="3"/>
+        <v>0.49999999999999023</v>
       </c>
       <c r="M8">
         <v>0.23699999999999999</v>
@@ -8723,10 +8858,14 @@
         <v>7.3269509706504598E-3</v>
       </c>
       <c r="O8">
+        <f t="shared" si="4"/>
+        <v>0.49999999999999023</v>
+      </c>
+      <c r="P8">
         <v>5.4999999999999902</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.45199999999999901</v>
       </c>
@@ -8734,7 +8873,8 @@
         <v>2.3753116139062402E-2</v>
       </c>
       <c r="C9">
-        <v>5.5999999999999899</v>
+        <f t="shared" si="0"/>
+        <v>0.59999999999998987</v>
       </c>
       <c r="D9">
         <v>0.41399999999999898</v>
@@ -8743,7 +8883,8 @@
         <v>5.0262468995003404E-3</v>
       </c>
       <c r="F9">
-        <v>5.5999999999999899</v>
+        <f t="shared" si="1"/>
+        <v>0.59999999999998987</v>
       </c>
       <c r="G9">
         <v>0.38700000000000001</v>
@@ -8752,7 +8893,8 @@
         <v>1.9761738683361601E-2</v>
       </c>
       <c r="I9">
-        <v>5.5999999999999899</v>
+        <f t="shared" si="2"/>
+        <v>0.59999999999998987</v>
       </c>
       <c r="J9">
         <v>0.39400000000000002</v>
@@ -8761,7 +8903,8 @@
         <v>8.8257995015808693E-3</v>
       </c>
       <c r="L9">
-        <v>5.5999999999999899</v>
+        <f t="shared" si="3"/>
+        <v>0.59999999999998987</v>
       </c>
       <c r="M9">
         <v>0.37</v>
@@ -8770,10 +8913,14 @@
         <v>0</v>
       </c>
       <c r="O9">
+        <f t="shared" si="4"/>
+        <v>0.59999999999998987</v>
+      </c>
+      <c r="P9">
         <v>5.5999999999999899</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.58399999999999896</v>
       </c>
@@ -8781,7 +8928,8 @@
         <v>5.9824304161611901E-3</v>
       </c>
       <c r="C10">
-        <v>5.6999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999041</v>
       </c>
       <c r="D10">
         <v>0.57750000000000001</v>
@@ -8790,7 +8938,8 @@
         <v>1.9967078166980599E-2</v>
       </c>
       <c r="F10">
-        <v>5.6999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>0.69999999999999041</v>
       </c>
       <c r="G10">
         <v>0.58149999999999902</v>
@@ -8799,7 +8948,8 @@
         <v>1.13670808176853E-2</v>
       </c>
       <c r="I10">
-        <v>5.6999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>0.69999999999999041</v>
       </c>
       <c r="J10">
         <v>0.57950000000000002</v>
@@ -8808,7 +8958,8 @@
         <v>1.1459310165698599E-2</v>
       </c>
       <c r="L10">
-        <v>5.6999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>0.69999999999999041</v>
       </c>
       <c r="M10">
         <v>0.51400000000000001</v>
@@ -8817,10 +8968,14 @@
         <v>5.0262468995003404E-3</v>
       </c>
       <c r="O10">
+        <f t="shared" si="4"/>
+        <v>0.69999999999999041</v>
+      </c>
+      <c r="P10">
         <v>5.6999999999999904</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.83149999999999902</v>
       </c>
@@ -8828,7 +8983,8 @@
         <v>4.7270219845168097E-2</v>
       </c>
       <c r="C11">
-        <v>5.7999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>0.79999999999999005</v>
       </c>
       <c r="D11">
         <v>0.76849999999999996</v>
@@ -8837,7 +8993,8 @@
         <v>1.7252002172135499E-2</v>
       </c>
       <c r="F11">
-        <v>5.7999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>0.79999999999999005</v>
       </c>
       <c r="G11">
         <v>0.84199999999999897</v>
@@ -8846,7 +9003,8 @@
         <v>9.0704842324170504E-2</v>
       </c>
       <c r="I11">
-        <v>5.7999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>0.79999999999999005</v>
       </c>
       <c r="J11">
         <v>0.77499999999999902</v>
@@ -8855,7 +9013,8 @@
         <v>2.8745709061939701E-2</v>
       </c>
       <c r="L11">
-        <v>5.7999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>0.79999999999999005</v>
       </c>
       <c r="M11">
         <v>0.70349999999999902</v>
@@ -8864,10 +9023,14 @@
         <v>1.8715318802914799E-2</v>
       </c>
       <c r="O11">
+        <f t="shared" si="4"/>
+        <v>0.79999999999999005</v>
+      </c>
+      <c r="P11">
         <v>5.7999999999999901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.03799999999999</v>
       </c>
@@ -8875,7 +9038,8 @@
         <v>3.2379330639029202E-2</v>
       </c>
       <c r="C12">
-        <v>5.8999999999999897</v>
+        <f t="shared" si="0"/>
+        <v>0.8999999999999897</v>
       </c>
       <c r="D12">
         <v>1.032</v>
@@ -8884,7 +9048,8 @@
         <v>2.8395700193404001E-2</v>
       </c>
       <c r="F12">
-        <v>5.8999999999999897</v>
+        <f t="shared" si="1"/>
+        <v>0.8999999999999897</v>
       </c>
       <c r="G12">
         <v>1.00599999999999</v>
@@ -8893,7 +9058,8 @@
         <v>2.7606254058779801E-2</v>
       </c>
       <c r="I12">
-        <v>5.8999999999999897</v>
+        <f t="shared" si="2"/>
+        <v>0.8999999999999897</v>
       </c>
       <c r="J12">
         <v>0.98199999999999998</v>
@@ -8902,7 +9068,8 @@
         <v>2.85804497036551E-2</v>
       </c>
       <c r="L12">
-        <v>5.8999999999999897</v>
+        <f t="shared" si="3"/>
+        <v>0.8999999999999897</v>
       </c>
       <c r="M12">
         <v>0.91049999999999898</v>
@@ -8911,10 +9078,14 @@
         <v>2.1392325234704301E-2</v>
       </c>
       <c r="O12">
+        <f t="shared" si="4"/>
+        <v>0.8999999999999897</v>
+      </c>
+      <c r="P12">
         <v>5.8999999999999897</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.3069999999999899</v>
       </c>
@@ -8922,7 +9093,8 @@
         <v>3.40433160608812E-2</v>
       </c>
       <c r="C13">
-        <v>5.9999999999999902</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999999023</v>
       </c>
       <c r="D13">
         <v>1.3320000000000001</v>
@@ -8931,7 +9103,8 @@
         <v>4.3480183023872701E-2</v>
       </c>
       <c r="F13">
-        <v>5.9999999999999902</v>
+        <f t="shared" si="1"/>
+        <v>0.99999999999999023</v>
       </c>
       <c r="G13">
         <v>1.2629999999999999</v>
@@ -8940,7 +9113,8 @@
         <v>4.0144475925940497E-2</v>
       </c>
       <c r="I13">
-        <v>5.9999999999999902</v>
+        <f t="shared" si="2"/>
+        <v>0.99999999999999023</v>
       </c>
       <c r="J13">
         <v>1.2309999999999901</v>
@@ -8949,7 +9123,8 @@
         <v>3.0418138632972502E-2</v>
       </c>
       <c r="L13">
-        <v>5.9999999999999902</v>
+        <f t="shared" si="3"/>
+        <v>0.99999999999999023</v>
       </c>
       <c r="M13">
         <v>1.16299999999999</v>
@@ -8958,10 +9133,14 @@
         <v>1.3416407864998699E-2</v>
       </c>
       <c r="O13">
+        <f t="shared" si="4"/>
+        <v>0.99999999999999023</v>
+      </c>
+      <c r="P13">
         <v>5.9999999999999902</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.6575</v>
       </c>
@@ -8969,7 +9148,8 @@
         <v>5.2503132738612998E-2</v>
       </c>
       <c r="C14">
-        <v>6.0999999999999899</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999899</v>
       </c>
       <c r="D14">
         <v>1.615</v>
@@ -8978,7 +9158,8 @@
         <v>1.8496087779795299E-2</v>
       </c>
       <c r="F14">
-        <v>6.0999999999999899</v>
+        <f t="shared" si="1"/>
+        <v>1.0999999999999899</v>
       </c>
       <c r="G14">
         <v>1.5640000000000001</v>
@@ -8987,7 +9168,8 @@
         <v>0.191294757404708</v>
       </c>
       <c r="I14">
-        <v>6.0999999999999899</v>
+        <f t="shared" si="2"/>
+        <v>1.0999999999999899</v>
       </c>
       <c r="J14">
         <v>1.6724999999999901</v>
@@ -8996,7 +9178,8 @@
         <v>0.12776932339180599</v>
       </c>
       <c r="L14">
-        <v>6.0999999999999899</v>
+        <f t="shared" si="3"/>
+        <v>1.0999999999999899</v>
       </c>
       <c r="M14">
         <v>1.4664999999999899</v>
@@ -9005,10 +9188,14 @@
         <v>9.8808693416808507E-3</v>
       </c>
       <c r="O14">
+        <f t="shared" si="4"/>
+        <v>1.0999999999999899</v>
+      </c>
+      <c r="P14">
         <v>6.0999999999999899</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.984</v>
       </c>
@@ -9016,7 +9203,8 @@
         <v>8.6169966681522797E-2</v>
       </c>
       <c r="C15">
-        <v>6.1999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>1.1999999999999904</v>
       </c>
       <c r="D15">
         <v>2.028</v>
@@ -9025,7 +9213,8 @@
         <v>0.22272475342779799</v>
       </c>
       <c r="F15">
-        <v>6.1999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>1.1999999999999904</v>
       </c>
       <c r="G15">
         <v>1.986</v>
@@ -9034,7 +9223,8 @@
         <v>0.13531250379846799</v>
       </c>
       <c r="I15">
-        <v>6.1999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>1.1999999999999904</v>
       </c>
       <c r="J15">
         <v>1.8804999999999901</v>
@@ -9043,7 +9233,8 @@
         <v>4.6393624788893403E-2</v>
       </c>
       <c r="L15">
-        <v>6.1999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>1.1999999999999904</v>
       </c>
       <c r="M15">
         <v>1.8299999999999901</v>
@@ -9052,10 +9243,14 @@
         <v>2.3841582427170799E-2</v>
       </c>
       <c r="O15">
+        <f t="shared" si="4"/>
+        <v>1.1999999999999904</v>
+      </c>
+      <c r="P15">
         <v>6.1999999999999904</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.3399999999999901</v>
       </c>
@@ -9063,7 +9258,8 @@
         <v>2.9199855803537299E-2</v>
       </c>
       <c r="C16">
-        <v>6.2999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>1.2999999999999901</v>
       </c>
       <c r="D16">
         <v>2.3259999999999899</v>
@@ -9072,7 +9268,8 @@
         <v>2.2803508501982799E-2</v>
       </c>
       <c r="F16">
-        <v>6.2999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>1.2999999999999901</v>
       </c>
       <c r="G16">
         <v>2.206</v>
@@ -9081,7 +9278,8 @@
         <v>6.3112264218112502E-2</v>
       </c>
       <c r="I16">
-        <v>6.2999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>1.2999999999999901</v>
       </c>
       <c r="J16">
         <v>2.2480000000000002</v>
@@ -9090,7 +9288,8 @@
         <v>4.1243819313673498E-2</v>
       </c>
       <c r="L16">
-        <v>6.2999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>1.2999999999999901</v>
       </c>
       <c r="M16">
         <v>2.20399999999999</v>
@@ -9099,10 +9298,14 @@
         <v>3.5894582496967101E-2</v>
       </c>
       <c r="O16">
+        <f t="shared" si="4"/>
+        <v>1.2999999999999901</v>
+      </c>
+      <c r="P16">
         <v>6.2999999999999901</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.8820000000000001</v>
       </c>
@@ -9110,7 +9313,8 @@
         <v>2.7834094957538399E-2</v>
       </c>
       <c r="C17">
-        <v>6.3999999999999897</v>
+        <f t="shared" si="0"/>
+        <v>1.3999999999999897</v>
       </c>
       <c r="D17">
         <v>2.9550000000000001</v>
@@ -9119,7 +9323,8 @@
         <v>0.57198178108636999</v>
       </c>
       <c r="F17">
-        <v>6.3999999999999897</v>
+        <f t="shared" si="1"/>
+        <v>1.3999999999999897</v>
       </c>
       <c r="G17">
         <v>2.7349999999999901</v>
@@ -9128,7 +9333,8 @@
         <v>5.1144789311172202E-2</v>
       </c>
       <c r="I17">
-        <v>6.3999999999999897</v>
+        <f t="shared" si="2"/>
+        <v>1.3999999999999897</v>
       </c>
       <c r="J17">
         <v>2.8039999999999998</v>
@@ -9137,7 +9343,8 @@
         <v>2.8727393858384201E-2</v>
       </c>
       <c r="L17">
-        <v>6.3999999999999897</v>
+        <f t="shared" si="3"/>
+        <v>1.3999999999999897</v>
       </c>
       <c r="M17">
         <v>2.6890000000000001</v>
@@ -9146,10 +9353,14 @@
         <v>2.6337885460422102E-2</v>
       </c>
       <c r="O17">
+        <f t="shared" si="4"/>
+        <v>1.3999999999999897</v>
+      </c>
+      <c r="P17">
         <v>6.3999999999999897</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.36899999999999</v>
       </c>
@@ -9157,7 +9368,8 @@
         <v>4.4117069139661597E-2</v>
       </c>
       <c r="C18">
-        <v>6.4999999999999902</v>
+        <f t="shared" si="0"/>
+        <v>1.4999999999999902</v>
       </c>
       <c r="D18">
         <v>3.395</v>
@@ -9166,7 +9378,8 @@
         <v>5.6054484772923303E-2</v>
       </c>
       <c r="F18">
-        <v>6.4999999999999902</v>
+        <f t="shared" si="1"/>
+        <v>1.4999999999999902</v>
       </c>
       <c r="G18">
         <v>3.1804999999999901</v>
@@ -9175,7 +9388,8 @@
         <v>7.1412441787865294E-2</v>
       </c>
       <c r="I18">
-        <v>6.4999999999999902</v>
+        <f t="shared" si="2"/>
+        <v>1.4999999999999902</v>
       </c>
       <c r="J18">
         <v>3.2634999999999899</v>
@@ -9184,7 +9398,8 @@
         <v>6.4012745441414706E-2</v>
       </c>
       <c r="L18">
-        <v>6.4999999999999902</v>
+        <f t="shared" si="3"/>
+        <v>1.4999999999999902</v>
       </c>
       <c r="M18">
         <v>3.1924999999999999</v>
@@ -9193,10 +9408,14 @@
         <v>6.1290936910512399E-2</v>
       </c>
       <c r="O18">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999902</v>
+      </c>
+      <c r="P18">
         <v>6.4999999999999902</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.8889999999999998</v>
       </c>
@@ -9204,7 +9423,8 @@
         <v>1.51830930903249E-2</v>
       </c>
       <c r="C19">
-        <v>6.5999999999999899</v>
+        <f t="shared" si="0"/>
+        <v>1.5999999999999899</v>
       </c>
       <c r="D19">
         <v>3.9289999999999998</v>
@@ -9213,7 +9433,8 @@
         <v>4.1409381088169703E-2</v>
       </c>
       <c r="F19">
-        <v>6.5999999999999899</v>
+        <f t="shared" si="1"/>
+        <v>1.5999999999999899</v>
       </c>
       <c r="G19">
         <v>3.6720000000000002</v>
@@ -9222,7 +9443,8 @@
         <v>2.2384204957490501E-2</v>
       </c>
       <c r="I19">
-        <v>6.5999999999999899</v>
+        <f t="shared" si="2"/>
+        <v>1.5999999999999899</v>
       </c>
       <c r="J19">
         <v>3.7639999999999998</v>
@@ -9231,7 +9453,8 @@
         <v>4.9989472575943897E-2</v>
       </c>
       <c r="L19">
-        <v>6.5999999999999899</v>
+        <f t="shared" si="3"/>
+        <v>1.5999999999999899</v>
       </c>
       <c r="M19">
         <v>3.6555</v>
@@ -9240,10 +9463,14 @@
         <v>2.4596747752497702E-2</v>
       </c>
       <c r="O19">
+        <f t="shared" si="4"/>
+        <v>1.5999999999999899</v>
+      </c>
+      <c r="P19">
         <v>6.5999999999999899</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.4260000000000002</v>
       </c>
@@ -9251,7 +9478,8 @@
         <v>5.03043369481148E-2</v>
       </c>
       <c r="C20">
-        <v>6.6999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>1.6999999999999904</v>
       </c>
       <c r="D20">
         <v>4.452</v>
@@ -9260,7 +9488,8 @@
         <v>8.2372708817269893E-2</v>
       </c>
       <c r="F20">
-        <v>6.6999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>1.6999999999999904</v>
       </c>
       <c r="G20">
         <v>4.18949999999999</v>
@@ -9269,7 +9498,8 @@
         <v>2.4596747752497702E-2</v>
       </c>
       <c r="I20">
-        <v>6.6999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>1.6999999999999904</v>
       </c>
       <c r="J20">
         <v>4.266</v>
@@ -9278,7 +9508,8 @@
         <v>4.0444894284497802E-2</v>
       </c>
       <c r="L20">
-        <v>6.6999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>1.6999999999999904</v>
       </c>
       <c r="M20">
         <v>4.1790000000000003</v>
@@ -9287,10 +9518,14 @@
         <v>4.6214602385871599E-2</v>
       </c>
       <c r="O20">
+        <f t="shared" si="4"/>
+        <v>1.6999999999999904</v>
+      </c>
+      <c r="P20">
         <v>6.6999999999999904</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.0090000000000003</v>
       </c>
@@ -9298,7 +9533,8 @@
         <v>4.99368021656003E-2</v>
       </c>
       <c r="C21">
-        <v>6.7999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>1.7999999999999901</v>
       </c>
       <c r="D21">
         <v>5.0134999999999899</v>
@@ -9307,7 +9543,8 @@
         <v>8.7676138505056594E-2</v>
       </c>
       <c r="F21">
-        <v>6.7999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>1.7999999999999901</v>
       </c>
       <c r="G21">
         <v>4.8149999999999897</v>
@@ -9316,7 +9553,8 @@
         <v>6.9774071492436099E-2</v>
       </c>
       <c r="I21">
-        <v>6.7999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>1.7999999999999901</v>
       </c>
       <c r="J21">
         <v>4.7939999999999996</v>
@@ -9325,7 +9563,8 @@
         <v>8.4567008622561696E-2</v>
       </c>
       <c r="L21">
-        <v>6.7999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>1.7999999999999901</v>
       </c>
       <c r="M21">
         <v>4.665</v>
@@ -9334,10 +9573,14 @@
         <v>5.1554774142092002E-2</v>
       </c>
       <c r="O21">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999901</v>
+      </c>
+      <c r="P21">
         <v>6.7999999999999901</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5.7</v>
       </c>
@@ -9345,7 +9588,8 @@
         <v>0.18081685994979901</v>
       </c>
       <c r="C22">
-        <v>6.8999999999999897</v>
+        <f t="shared" si="0"/>
+        <v>1.8999999999999897</v>
       </c>
       <c r="D22">
         <v>5.6050000000000004</v>
@@ -9354,7 +9598,8 @@
         <v>0.105805183436849</v>
       </c>
       <c r="F22">
-        <v>6.8999999999999897</v>
+        <f t="shared" si="1"/>
+        <v>1.8999999999999897</v>
       </c>
       <c r="G22">
         <v>5.3239999999999901</v>
@@ -9363,7 +9608,8 @@
         <v>0.10624698138126799</v>
       </c>
       <c r="I22">
-        <v>6.8999999999999897</v>
+        <f t="shared" si="2"/>
+        <v>1.8999999999999897</v>
       </c>
       <c r="J22">
         <v>5.4869999999999903</v>
@@ -9372,7 +9618,8 @@
         <v>0.51658901510418798</v>
       </c>
       <c r="L22">
-        <v>6.8999999999999897</v>
+        <f t="shared" si="3"/>
+        <v>1.8999999999999897</v>
       </c>
       <c r="M22">
         <v>5.1989999999999901</v>
@@ -9381,10 +9628,14 @@
         <v>4.5526163674829499E-2</v>
       </c>
       <c r="O22">
+        <f t="shared" si="4"/>
+        <v>1.8999999999999897</v>
+      </c>
+      <c r="P22">
         <v>6.8999999999999897</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.2039999999999997</v>
       </c>
@@ -9392,7 +9643,8 @@
         <v>3.84433965310313E-2</v>
       </c>
       <c r="C23">
-        <v>6.9999999999999902</v>
+        <f t="shared" si="0"/>
+        <v>1.9999999999999902</v>
       </c>
       <c r="D23">
         <v>6.2179999999999902</v>
@@ -9401,7 +9653,8 @@
         <v>0.116148724985638</v>
       </c>
       <c r="F23">
-        <v>6.9999999999999902</v>
+        <f t="shared" si="1"/>
+        <v>1.9999999999999902</v>
       </c>
       <c r="G23">
         <v>6.0449999999999902</v>
@@ -9410,7 +9663,8 @@
         <v>0.116641601317431</v>
       </c>
       <c r="I23">
-        <v>6.9999999999999902</v>
+        <f t="shared" si="2"/>
+        <v>1.9999999999999902</v>
       </c>
       <c r="J23">
         <v>5.9269999999999996</v>
@@ -9419,7 +9673,8 @@
         <v>7.1237187213598202E-2</v>
       </c>
       <c r="L23">
-        <v>6.9999999999999902</v>
+        <f t="shared" si="3"/>
+        <v>1.9999999999999902</v>
       </c>
       <c r="M23">
         <v>5.8049999999999899</v>
@@ -9428,10 +9683,14 @@
         <v>4.1612245161351501E-2</v>
       </c>
       <c r="O23">
+        <f t="shared" si="4"/>
+        <v>1.9999999999999902</v>
+      </c>
+      <c r="P23">
         <v>6.9999999999999902</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6.8224999999999998</v>
       </c>
@@ -9439,7 +9698,8 @@
         <v>6.3068467390189301E-2</v>
       </c>
       <c r="C24">
-        <v>7.0999999999999899</v>
+        <f t="shared" si="0"/>
+        <v>2.0999999999999899</v>
       </c>
       <c r="D24">
         <v>6.8220000000000001</v>
@@ -9448,7 +9708,8 @@
         <v>0.13008499245938299</v>
       </c>
       <c r="F24">
-        <v>7.0999999999999899</v>
+        <f t="shared" si="1"/>
+        <v>2.0999999999999899</v>
       </c>
       <c r="G24">
         <v>6.82899999999999</v>
@@ -9457,7 +9718,8 @@
         <v>0.34494698295916598</v>
       </c>
       <c r="I24">
-        <v>7.0999999999999899</v>
+        <f t="shared" si="2"/>
+        <v>2.0999999999999899</v>
       </c>
       <c r="J24">
         <v>6.6704999999999899</v>
@@ -9466,7 +9728,8 @@
         <v>0.13124805762973701</v>
       </c>
       <c r="L24">
-        <v>7.0999999999999899</v>
+        <f t="shared" si="3"/>
+        <v>2.0999999999999899</v>
       </c>
       <c r="M24">
         <v>6.4189999999999898</v>
@@ -9475,10 +9738,14 @@
         <v>4.74508055502584E-2</v>
       </c>
       <c r="O24">
+        <f t="shared" si="4"/>
+        <v>2.0999999999999899</v>
+      </c>
+      <c r="P24">
         <v>7.0999999999999899</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7.585</v>
       </c>
@@ -9486,7 +9753,8 @@
         <v>9.5504202167124297E-2</v>
       </c>
       <c r="C25">
-        <v>7.1999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>2.1999999999999904</v>
       </c>
       <c r="D25">
         <v>7.5270000000000001</v>
@@ -9495,7 +9763,8 @@
         <v>0.15543148769931001</v>
       </c>
       <c r="F25">
-        <v>7.1999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>2.1999999999999904</v>
       </c>
       <c r="G25">
         <v>7.3220000000000001</v>
@@ -9504,7 +9773,8 @@
         <v>0.42584405349228099</v>
       </c>
       <c r="I25">
-        <v>7.1999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>2.1999999999999904</v>
       </c>
       <c r="J25">
         <v>7.2939999999999898</v>
@@ -9513,7 +9783,8 @@
         <v>0.128325244675599</v>
       </c>
       <c r="L25">
-        <v>7.1999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>2.1999999999999904</v>
       </c>
       <c r="M25">
         <v>7.0309999999999899</v>
@@ -9522,10 +9793,14 @@
         <v>2.4899799195977401E-2</v>
       </c>
       <c r="O25">
+        <f t="shared" si="4"/>
+        <v>2.1999999999999904</v>
+      </c>
+      <c r="P25">
         <v>7.1999999999999904</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8.3390000000000004</v>
       </c>
@@ -9533,7 +9808,8 @@
         <v>3.2101811721294803E-2</v>
       </c>
       <c r="C26">
-        <v>7.2999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>2.2999999999999901</v>
       </c>
       <c r="D26">
         <v>8.2434999999999903</v>
@@ -9542,7 +9818,8 @@
         <v>5.4606246027933E-2</v>
       </c>
       <c r="F26">
-        <v>7.2999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>2.2999999999999901</v>
       </c>
       <c r="G26">
         <v>8.1359999999999904</v>
@@ -9551,7 +9828,8 @@
         <v>0.37055292966620901</v>
       </c>
       <c r="I26">
-        <v>7.2999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>2.2999999999999901</v>
       </c>
       <c r="J26">
         <v>7.9335000000000004</v>
@@ -9560,7 +9838,8 @@
         <v>7.6314791282038094E-2</v>
       </c>
       <c r="L26">
-        <v>7.2999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>2.2999999999999901</v>
       </c>
       <c r="M26">
         <v>7.7779999999999996</v>
@@ -9569,10 +9848,14 @@
         <v>3.3654592241585103E-2</v>
       </c>
       <c r="O26">
+        <f t="shared" si="4"/>
+        <v>2.2999999999999901</v>
+      </c>
+      <c r="P26">
         <v>7.2999999999999901</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9.1144999999999907</v>
       </c>
@@ -9580,7 +9863,8 @@
         <v>0.449683807042003</v>
       </c>
       <c r="C27">
-        <v>7.3999999999999897</v>
+        <f t="shared" si="0"/>
+        <v>2.3999999999999897</v>
       </c>
       <c r="D27">
         <v>8.98</v>
@@ -9589,7 +9873,8 @@
         <v>9.1651513899116896E-2</v>
       </c>
       <c r="F27">
-        <v>7.3999999999999897</v>
+        <f t="shared" si="1"/>
+        <v>2.3999999999999897</v>
       </c>
       <c r="G27">
         <v>9.0860000000000003</v>
@@ -9598,7 +9883,8 @@
         <v>0.38383658803687398</v>
       </c>
       <c r="I27">
-        <v>7.3999999999999897</v>
+        <f t="shared" si="2"/>
+        <v>2.3999999999999897</v>
       </c>
       <c r="J27">
         <v>8.6590000000000007</v>
@@ -9607,7 +9893,8 @@
         <v>0.111208670619932</v>
       </c>
       <c r="L27">
-        <v>7.3999999999999897</v>
+        <f t="shared" si="3"/>
+        <v>2.3999999999999897</v>
       </c>
       <c r="M27">
         <v>8.532</v>
@@ -9616,10 +9903,14 @@
         <v>6.59026395126696E-2</v>
       </c>
       <c r="O27">
+        <f t="shared" si="4"/>
+        <v>2.3999999999999897</v>
+      </c>
+      <c r="P27">
         <v>7.3999999999999897</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10.063999999999901</v>
       </c>
@@ -9627,7 +9918,8 @@
         <v>0.49939331614522597</v>
       </c>
       <c r="C28">
-        <v>7.4999999999999902</v>
+        <f t="shared" si="0"/>
+        <v>2.4999999999999902</v>
       </c>
       <c r="D28">
         <v>10.077999999999999</v>
@@ -9636,7 +9928,8 @@
         <v>0.13881452980221601</v>
       </c>
       <c r="F28">
-        <v>7.4999999999999902</v>
+        <f t="shared" si="1"/>
+        <v>2.4999999999999902</v>
       </c>
       <c r="G28">
         <v>9.5489999999999906</v>
@@ -9645,7 +9938,8 @@
         <v>0.48128009133537702</v>
       </c>
       <c r="I28">
-        <v>7.4999999999999902</v>
+        <f t="shared" si="2"/>
+        <v>2.4999999999999902</v>
       </c>
       <c r="J28">
         <v>9.5310000000000006</v>
@@ -9654,7 +9948,8 @@
         <v>0.56049695994292703</v>
       </c>
       <c r="L28">
-        <v>7.4999999999999902</v>
+        <f t="shared" si="3"/>
+        <v>2.4999999999999902</v>
       </c>
       <c r="M28">
         <v>9.1880000000000006</v>
@@ -9663,10 +9958,14 @@
         <v>4.6066313756994701E-2</v>
       </c>
       <c r="O28">
+        <f t="shared" si="4"/>
+        <v>2.4999999999999902</v>
+      </c>
+      <c r="P28">
         <v>7.4999999999999902</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10.63</v>
       </c>
@@ -9674,7 +9973,8 @@
         <v>7.3125702875614096E-2</v>
       </c>
       <c r="C29">
-        <v>7.5999999999999899</v>
+        <f t="shared" si="0"/>
+        <v>2.5999999999999899</v>
       </c>
       <c r="D29">
         <v>10.611000000000001</v>
@@ -9683,7 +9983,8 @@
         <v>0.10627174700044301</v>
       </c>
       <c r="F29">
-        <v>7.5999999999999899</v>
+        <f t="shared" si="1"/>
+        <v>2.5999999999999899</v>
       </c>
       <c r="G29">
         <v>10.2259999999999</v>
@@ -9692,7 +9993,8 @@
         <v>0.28907110762433103</v>
       </c>
       <c r="I29">
-        <v>7.5999999999999899</v>
+        <f t="shared" si="2"/>
+        <v>2.5999999999999899</v>
       </c>
       <c r="J29">
         <v>10.0985</v>
@@ -9701,7 +10003,8 @@
         <v>6.5475989974630402E-2</v>
       </c>
       <c r="L29">
-        <v>7.5999999999999899</v>
+        <f t="shared" si="3"/>
+        <v>2.5999999999999899</v>
       </c>
       <c r="M29">
         <v>9.9060000000000006</v>
@@ -9710,10 +10013,14 @@
         <v>4.2227454277245502E-2</v>
       </c>
       <c r="O29">
+        <f t="shared" si="4"/>
+        <v>2.5999999999999899</v>
+      </c>
+      <c r="P29">
         <v>7.5999999999999899</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11.375999999999999</v>
       </c>
@@ -9721,7 +10028,8 @@
         <v>6.9312412498165096E-2</v>
       </c>
       <c r="C30">
-        <v>7.6999999999999904</v>
+        <f t="shared" si="0"/>
+        <v>2.6999999999999904</v>
       </c>
       <c r="D30">
         <v>11.312999999999899</v>
@@ -9730,7 +10038,8 @@
         <v>9.2798593455765396E-2</v>
       </c>
       <c r="F30">
-        <v>7.6999999999999904</v>
+        <f t="shared" si="1"/>
+        <v>2.6999999999999904</v>
       </c>
       <c r="G30">
         <v>10.791</v>
@@ -9739,7 +10048,8 @@
         <v>0.331248038723091</v>
       </c>
       <c r="I30">
-        <v>7.6999999999999904</v>
+        <f t="shared" si="2"/>
+        <v>2.6999999999999904</v>
       </c>
       <c r="J30">
         <v>10.789</v>
@@ -9748,7 +10058,8 @@
         <v>6.8356649851695803E-2</v>
       </c>
       <c r="L30">
-        <v>7.6999999999999904</v>
+        <f t="shared" si="3"/>
+        <v>2.6999999999999904</v>
       </c>
       <c r="M30">
         <v>10.6229999999999</v>
@@ -9757,10 +10068,14 @@
         <v>6.5542272417762407E-2</v>
       </c>
       <c r="O30">
+        <f t="shared" si="4"/>
+        <v>2.6999999999999904</v>
+      </c>
+      <c r="P30">
         <v>7.6999999999999904</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12.1455</v>
       </c>
@@ -9768,7 +10083,8 @@
         <v>5.67983506061479E-2</v>
       </c>
       <c r="C31">
-        <v>7.7999999999999901</v>
+        <f t="shared" si="0"/>
+        <v>2.7999999999999901</v>
       </c>
       <c r="D31">
         <v>12.026</v>
@@ -9777,7 +10093,8 @@
         <v>0.154966889502581</v>
       </c>
       <c r="F31">
-        <v>7.7999999999999901</v>
+        <f t="shared" si="1"/>
+        <v>2.7999999999999901</v>
       </c>
       <c r="G31">
         <v>11.611000000000001</v>
@@ -9786,7 +10103,8 @@
         <v>0.245290375720395</v>
       </c>
       <c r="I31">
-        <v>7.7999999999999901</v>
+        <f t="shared" si="2"/>
+        <v>2.7999999999999901</v>
       </c>
       <c r="J31">
         <v>11.5745</v>
@@ -9795,7 +10113,8 @@
         <v>4.8825683491591401E-2</v>
       </c>
       <c r="L31">
-        <v>7.7999999999999901</v>
+        <f t="shared" si="3"/>
+        <v>2.7999999999999901</v>
       </c>
       <c r="M31">
         <v>11.2919999999999</v>
@@ -9804,10 +10123,14 @@
         <v>7.4240009074409405E-2</v>
       </c>
       <c r="O31">
+        <f t="shared" si="4"/>
+        <v>2.7999999999999901</v>
+      </c>
+      <c r="P31">
         <v>7.7999999999999901</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12.9305</v>
       </c>
@@ -9815,7 +10138,8 @@
         <v>5.0520970111950801E-2</v>
       </c>
       <c r="C32">
-        <v>7.8999999999999799</v>
+        <f t="shared" si="0"/>
+        <v>2.8999999999999799</v>
       </c>
       <c r="D32">
         <v>12.693</v>
@@ -9824,7 +10148,8 @@
         <v>6.2247384218979497E-2</v>
       </c>
       <c r="F32">
-        <v>7.8999999999999799</v>
+        <f t="shared" si="1"/>
+        <v>2.8999999999999799</v>
       </c>
       <c r="G32">
         <v>12.269499999999899</v>
@@ -9833,7 +10158,8 @@
         <v>4.6393624788893299E-2</v>
       </c>
       <c r="I32">
-        <v>7.8999999999999799</v>
+        <f t="shared" si="2"/>
+        <v>2.8999999999999799</v>
       </c>
       <c r="J32">
         <v>12.298</v>
@@ -9842,7 +10168,8 @@
         <v>0.15140047973225801</v>
       </c>
       <c r="L32">
-        <v>7.8999999999999799</v>
+        <f t="shared" si="3"/>
+        <v>2.8999999999999799</v>
       </c>
       <c r="M32">
         <v>11.928000000000001</v>
@@ -9851,10 +10178,14 @@
         <v>9.33358395653483E-2</v>
       </c>
       <c r="O32">
+        <f t="shared" si="4"/>
+        <v>2.8999999999999799</v>
+      </c>
+      <c r="P32">
         <v>7.8999999999999799</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>13.625</v>
       </c>
@@ -9862,7 +10193,8 @@
         <v>9.0291924217769201E-2</v>
       </c>
       <c r="C33">
-        <v>7.9999999999999796</v>
+        <f t="shared" si="0"/>
+        <v>2.9999999999999796</v>
       </c>
       <c r="D33">
         <v>13.388499999999899</v>
@@ -9871,7 +10203,8 @@
         <v>0.119087539672558</v>
       </c>
       <c r="F33">
-        <v>7.9999999999999796</v>
+        <f t="shared" si="1"/>
+        <v>2.9999999999999796</v>
       </c>
       <c r="G33">
         <v>13.0214999999999</v>
@@ -9880,7 +10213,8 @@
         <v>7.22040237980653E-2</v>
       </c>
       <c r="I33">
-        <v>7.9999999999999796</v>
+        <f t="shared" si="2"/>
+        <v>2.9999999999999796</v>
       </c>
       <c r="J33">
         <v>13.055</v>
@@ -9889,7 +10223,8 @@
         <v>0.110905365064094</v>
       </c>
       <c r="L33">
-        <v>7.9999999999999796</v>
+        <f t="shared" si="3"/>
+        <v>2.9999999999999796</v>
       </c>
       <c r="M33">
         <v>12.7754999999999</v>
@@ -9898,10 +10233,14 @@
         <v>6.6052212202484695E-2</v>
       </c>
       <c r="O33">
+        <f t="shared" si="4"/>
+        <v>2.9999999999999796</v>
+      </c>
+      <c r="P33">
         <v>7.9999999999999796</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14.3529999999999</v>
       </c>
@@ -9909,7 +10248,8 @@
         <v>0.13479419009812799</v>
       </c>
       <c r="C34">
-        <v>8.0999999999999801</v>
+        <f t="shared" si="0"/>
+        <v>3.0999999999999801</v>
       </c>
       <c r="D34">
         <v>14.031000000000001</v>
@@ -9918,7 +10258,8 @@
         <v>0.13206457750501799</v>
       </c>
       <c r="F34">
-        <v>8.0999999999999801</v>
+        <f t="shared" si="1"/>
+        <v>3.0999999999999801</v>
       </c>
       <c r="G34">
         <v>13.7319999999999</v>
@@ -9927,7 +10268,8 @@
         <v>0.17270601732728499</v>
       </c>
       <c r="I34">
-        <v>8.0999999999999801</v>
+        <f t="shared" si="2"/>
+        <v>3.0999999999999801</v>
       </c>
       <c r="J34">
         <v>13.6474999999999</v>
@@ -9936,7 +10278,8 @@
         <v>0.34979505277714801</v>
       </c>
       <c r="L34">
-        <v>8.0999999999999801</v>
+        <f t="shared" si="3"/>
+        <v>3.0999999999999801</v>
       </c>
       <c r="M34">
         <v>13.4565</v>
@@ -9945,10 +10288,14 @@
         <v>0.103072534500811</v>
       </c>
       <c r="O34">
+        <f t="shared" si="4"/>
+        <v>3.0999999999999801</v>
+      </c>
+      <c r="P34">
         <v>8.0999999999999801</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15.129</v>
       </c>
@@ -9956,7 +10303,8 @@
         <v>0.100572048015863</v>
       </c>
       <c r="C35">
-        <v>8.1999999999999797</v>
+        <f t="shared" si="0"/>
+        <v>3.1999999999999797</v>
       </c>
       <c r="D35">
         <v>14.619</v>
@@ -9965,7 +10313,8 @@
         <v>7.3906057012655693E-2</v>
       </c>
       <c r="F35">
-        <v>8.1999999999999797</v>
+        <f t="shared" si="1"/>
+        <v>3.1999999999999797</v>
       </c>
       <c r="G35">
         <v>14.337</v>
@@ -9974,7 +10323,8 @@
         <v>0.14179674111020199</v>
       </c>
       <c r="I35">
-        <v>8.1999999999999797</v>
+        <f t="shared" si="2"/>
+        <v>3.1999999999999797</v>
       </c>
       <c r="J35">
         <v>14.5145</v>
@@ -9983,7 +10333,8 @@
         <v>0.21905238498683499</v>
       </c>
       <c r="L35">
-        <v>8.1999999999999797</v>
+        <f t="shared" si="3"/>
+        <v>3.1999999999999797</v>
       </c>
       <c r="M35">
         <v>13.9659999999999</v>
@@ -9992,10 +10343,14 @@
         <v>0.12700600897512401</v>
       </c>
       <c r="O35">
+        <f t="shared" si="4"/>
+        <v>3.1999999999999797</v>
+      </c>
+      <c r="P35">
         <v>8.1999999999999797</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>16.096499999999999</v>
       </c>
@@ -10003,7 +10358,8 @@
         <v>0.10291923251294</v>
       </c>
       <c r="C36">
-        <v>8.2999999999999794</v>
+        <f t="shared" si="0"/>
+        <v>3.2999999999999794</v>
       </c>
       <c r="D36">
         <v>15.4734999999999</v>
@@ -10012,7 +10368,8 @@
         <v>0.15260113126434499</v>
       </c>
       <c r="F36">
-        <v>8.2999999999999794</v>
+        <f t="shared" si="1"/>
+        <v>3.2999999999999794</v>
       </c>
       <c r="G36">
         <v>15.136999999999899</v>
@@ -10021,7 +10378,8 @@
         <v>9.79312325858787E-2</v>
       </c>
       <c r="I36">
-        <v>8.2999999999999794</v>
+        <f t="shared" si="2"/>
+        <v>3.2999999999999794</v>
       </c>
       <c r="J36">
         <v>14.993</v>
@@ -10030,7 +10388,8 @@
         <v>0.17311693644531301</v>
       </c>
       <c r="L36">
-        <v>8.2999999999999794</v>
+        <f t="shared" si="3"/>
+        <v>3.2999999999999794</v>
       </c>
       <c r="M36">
         <v>14.6204999999999</v>
@@ -10039,10 +10398,14 @@
         <v>0.116052392886733</v>
       </c>
       <c r="O36">
+        <f t="shared" si="4"/>
+        <v>3.2999999999999794</v>
+      </c>
+      <c r="P36">
         <v>8.2999999999999794</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16.943000000000001</v>
       </c>
@@ -10050,7 +10413,8 @@
         <v>0.124439797323423</v>
       </c>
       <c r="C37">
-        <v>8.3999999999999808</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999999808</v>
       </c>
       <c r="D37">
         <v>16.0945</v>
@@ -10059,7 +10423,8 @@
         <v>0.169441031506228</v>
       </c>
       <c r="F37">
-        <v>8.3999999999999808</v>
+        <f t="shared" si="1"/>
+        <v>3.3999999999999808</v>
       </c>
       <c r="G37">
         <v>15.811</v>
@@ -10068,7 +10433,8 @@
         <v>0.12565198387861401</v>
       </c>
       <c r="I37">
-        <v>8.3999999999999808</v>
+        <f t="shared" si="2"/>
+        <v>3.3999999999999808</v>
       </c>
       <c r="J37">
         <v>15.550999999999901</v>
@@ -10077,7 +10443,8 @@
         <v>0.136532240264264</v>
       </c>
       <c r="L37">
-        <v>8.3999999999999808</v>
+        <f t="shared" si="3"/>
+        <v>3.3999999999999808</v>
       </c>
       <c r="M37">
         <v>15.3055</v>
@@ -10086,7 +10453,19 @@
         <v>0.174551304477327</v>
       </c>
       <c r="O37">
+        <f t="shared" si="4"/>
+        <v>3.3999999999999808</v>
+      </c>
+      <c r="P37">
         <v>8.3999999999999808</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified calculation of thrust constant to be based on pulse width rather than duty  cycle
</commit_message>
<xml_diff>
--- a/tests/rotor3/Rotor3_Thrust_Constant_Calculation.xlsx
+++ b/tests/rotor3/Rotor3_Thrust_Constant_Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fer\repos\rx-2\tests\rotor3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA63C240-E4ED-4C8B-9AE0-1C5DE88CB810}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50DC8A8-14C8-4025-A100-56BA6F0B4BF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Force {N} (mean)</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>offset</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>offset t (ms)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -614,6 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,7 +999,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$C$3:$C$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1000,106 +1007,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1263,7 +1270,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$C$3:$C$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1271,106 +1278,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1866,7 +1873,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$I$3:$I$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1874,106 +1881,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2137,7 +2144,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$I$3:$I$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -2145,106 +2152,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2733,7 +2740,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$F$3:$F$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -2741,106 +2748,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3004,7 +3011,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$F$3:$F$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -3012,106 +3019,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3607,7 +3614,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$L$3:$L$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -3615,106 +3622,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3878,7 +3885,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$L$3:$L$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -3886,106 +3893,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4489,7 +4496,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$O$3:$O$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -4497,106 +4504,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4760,7 +4767,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Rotor2!$O$3:$O$37</c:f>
+              <c:f>Rotor2!$Q$3:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -4768,106 +4775,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999989875E-2</c:v>
+                  <c:v>1.9999999999997884E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999041</c:v>
+                  <c:v>3.9999999999998155E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999005</c:v>
+                  <c:v>5.9999999999997986E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3999999999999897</c:v>
+                  <c:v>7.9999999999997823E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49999999999999023</c:v>
+                  <c:v>9.999999999999809E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59999999999998987</c:v>
+                  <c:v>0.11999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69999999999999041</c:v>
+                  <c:v>0.13999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999005</c:v>
+                  <c:v>0.15999999999999803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8999999999999897</c:v>
+                  <c:v>0.17999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999023</c:v>
+                  <c:v>0.19999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0999999999999899</c:v>
+                  <c:v>0.21999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1999999999999904</c:v>
+                  <c:v>0.23999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2999999999999901</c:v>
+                  <c:v>0.25999999999999807</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3999999999999897</c:v>
+                  <c:v>0.27999999999999792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4999999999999902</c:v>
+                  <c:v>0.29999999999999799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5999999999999899</c:v>
+                  <c:v>0.31999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6999999999999904</c:v>
+                  <c:v>0.33999999999999808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7999999999999901</c:v>
+                  <c:v>0.35999999999999793</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8999999999999897</c:v>
+                  <c:v>0.37999999999999795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9999999999999902</c:v>
+                  <c:v>0.39999999999999802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0999999999999899</c:v>
+                  <c:v>0.41999999999999788</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1999999999999904</c:v>
+                  <c:v>0.43999999999999811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999901</c:v>
+                  <c:v>0.45999999999999797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3999999999999897</c:v>
+                  <c:v>0.47999999999999798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4999999999999902</c:v>
+                  <c:v>0.49999999999999806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5999999999999899</c:v>
+                  <c:v>0.51999999999999791</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6999999999999904</c:v>
+                  <c:v>0.53999999999999815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7999999999999901</c:v>
+                  <c:v>0.55999999999999805</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.8999999999999799</c:v>
+                  <c:v>0.57999999999999585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9999999999999796</c:v>
+                  <c:v>0.59999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0999999999999801</c:v>
+                  <c:v>0.619999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.1999999999999797</c:v>
+                  <c:v>0.63999999999999579</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2999999999999794</c:v>
+                  <c:v>0.65999999999999592</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3999999999999808</c:v>
+                  <c:v>0.67999999999999616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7975,16 +7982,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8011,16 +8018,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8047,16 +8054,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>90486</xdr:rowOff>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8083,16 +8090,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>157162</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8119,16 +8126,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8453,15 +8460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -8488,7 +8495,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8535,7 +8542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -8589,8 +8596,12 @@
       <c r="P3">
         <v>5</v>
       </c>
+      <c r="Q3">
+        <f>(((P3)/(100*$B$39)) -$B$40)*1000</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -8644,8 +8655,12 @@
       <c r="P4">
         <v>5.0999999999999899</v>
       </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q37" si="5">(((P4)/(100*$B$39)) -$B$40)*1000</f>
+        <v>1.9999999999997884E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -8699,8 +8714,12 @@
       <c r="P5">
         <v>5.1999999999999904</v>
       </c>
+      <c r="Q5">
+        <f t="shared" si="5"/>
+        <v>3.9999999999998155E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -8754,8 +8773,12 @@
       <c r="P6">
         <v>5.2999999999999901</v>
       </c>
+      <c r="Q6">
+        <f t="shared" si="5"/>
+        <v>5.9999999999997986E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.127999999999999</v>
       </c>
@@ -8809,8 +8832,12 @@
       <c r="P7">
         <v>5.3999999999999897</v>
       </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>7.9999999999997823E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.28399999999999997</v>
       </c>
@@ -8864,8 +8891,12 @@
       <c r="P8">
         <v>5.4999999999999902</v>
       </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>9.999999999999809E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.45199999999999901</v>
       </c>
@@ -8919,8 +8950,12 @@
       <c r="P9">
         <v>5.5999999999999899</v>
       </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>0.11999999999999793</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.58399999999999896</v>
       </c>
@@ -8974,8 +9009,12 @@
       <c r="P10">
         <v>5.6999999999999904</v>
       </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>0.13999999999999799</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.83149999999999902</v>
       </c>
@@ -9029,8 +9068,12 @@
       <c r="P11">
         <v>5.7999999999999901</v>
       </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>0.15999999999999803</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.03799999999999</v>
       </c>
@@ -9084,8 +9127,12 @@
       <c r="P12">
         <v>5.8999999999999897</v>
       </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>0.17999999999999788</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.3069999999999899</v>
       </c>
@@ -9139,8 +9186,12 @@
       <c r="P13">
         <v>5.9999999999999902</v>
       </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>0.19999999999999793</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.6575</v>
       </c>
@@ -9194,8 +9245,12 @@
       <c r="P14">
         <v>6.0999999999999899</v>
       </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.21999999999999797</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.984</v>
       </c>
@@ -9249,8 +9304,12 @@
       <c r="P15">
         <v>6.1999999999999904</v>
       </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>0.23999999999999802</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.3399999999999901</v>
       </c>
@@ -9304,8 +9363,12 @@
       <c r="P16">
         <v>6.2999999999999901</v>
       </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>0.25999999999999807</v>
+      </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.8820000000000001</v>
       </c>
@@ -9359,8 +9422,12 @@
       <c r="P17">
         <v>6.3999999999999897</v>
       </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>0.27999999999999792</v>
+      </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.36899999999999</v>
       </c>
@@ -9414,8 +9481,12 @@
       <c r="P18">
         <v>6.4999999999999902</v>
       </c>
+      <c r="Q18">
+        <f t="shared" si="5"/>
+        <v>0.29999999999999799</v>
+      </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.8889999999999998</v>
       </c>
@@ -9469,8 +9540,12 @@
       <c r="P19">
         <v>6.5999999999999899</v>
       </c>
+      <c r="Q19">
+        <f t="shared" si="5"/>
+        <v>0.31999999999999801</v>
+      </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.4260000000000002</v>
       </c>
@@ -9524,8 +9599,12 @@
       <c r="P20">
         <v>6.6999999999999904</v>
       </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>0.33999999999999808</v>
+      </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.0090000000000003</v>
       </c>
@@ -9579,8 +9658,12 @@
       <c r="P21">
         <v>6.7999999999999901</v>
       </c>
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>0.35999999999999793</v>
+      </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5.7</v>
       </c>
@@ -9634,8 +9717,12 @@
       <c r="P22">
         <v>6.8999999999999897</v>
       </c>
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>0.37999999999999795</v>
+      </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.2039999999999997</v>
       </c>
@@ -9689,8 +9776,12 @@
       <c r="P23">
         <v>6.9999999999999902</v>
       </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>0.39999999999999802</v>
+      </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6.8224999999999998</v>
       </c>
@@ -9744,8 +9835,12 @@
       <c r="P24">
         <v>7.0999999999999899</v>
       </c>
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>0.41999999999999788</v>
+      </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7.585</v>
       </c>
@@ -9799,8 +9894,12 @@
       <c r="P25">
         <v>7.1999999999999904</v>
       </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>0.43999999999999811</v>
+      </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8.3390000000000004</v>
       </c>
@@ -9854,8 +9953,12 @@
       <c r="P26">
         <v>7.2999999999999901</v>
       </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>0.45999999999999797</v>
+      </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9.1144999999999907</v>
       </c>
@@ -9909,8 +10012,12 @@
       <c r="P27">
         <v>7.3999999999999897</v>
       </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>0.47999999999999798</v>
+      </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10.063999999999901</v>
       </c>
@@ -9964,8 +10071,12 @@
       <c r="P28">
         <v>7.4999999999999902</v>
       </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>0.49999999999999806</v>
+      </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10.63</v>
       </c>
@@ -10019,8 +10130,12 @@
       <c r="P29">
         <v>7.5999999999999899</v>
       </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>0.51999999999999791</v>
+      </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11.375999999999999</v>
       </c>
@@ -10074,8 +10189,12 @@
       <c r="P30">
         <v>7.6999999999999904</v>
       </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>0.53999999999999815</v>
+      </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12.1455</v>
       </c>
@@ -10129,8 +10248,12 @@
       <c r="P31">
         <v>7.7999999999999901</v>
       </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>0.55999999999999805</v>
+      </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12.9305</v>
       </c>
@@ -10184,8 +10307,12 @@
       <c r="P32">
         <v>7.8999999999999799</v>
       </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>0.57999999999999585</v>
+      </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>13.625</v>
       </c>
@@ -10239,8 +10366,12 @@
       <c r="P33">
         <v>7.9999999999999796</v>
       </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>0.59999999999999598</v>
+      </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14.3529999999999</v>
       </c>
@@ -10294,8 +10425,12 @@
       <c r="P34">
         <v>8.0999999999999801</v>
       </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>0.619999999999996</v>
+      </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15.129</v>
       </c>
@@ -10349,8 +10484,12 @@
       <c r="P35">
         <v>8.1999999999999797</v>
       </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>0.63999999999999579</v>
+      </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>16.096499999999999</v>
       </c>
@@ -10404,8 +10543,12 @@
       <c r="P36">
         <v>8.2999999999999794</v>
       </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>0.65999999999999592</v>
+      </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16.943000000000001</v>
       </c>
@@ -10459,13 +10602,33 @@
       <c r="P37">
         <v>8.3999999999999808</v>
       </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>0.67999999999999616</v>
+      </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
       <c r="B38">
         <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>